<commit_message>
moved staging files StagingTemplates directory
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Activity.xlsx
+++ b/StagingTemplates/Staging.Activity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,19 +32,19 @@
     <t>Activity_ID</t>
   </si>
   <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>LongName</t>
+  </si>
+  <si>
+    <t>ProjectBusinessKey</t>
+  </si>
+  <si>
     <t>ShortName</t>
   </si>
   <si>
-    <t>LongName</t>
-  </si>
-  <si>
     <t>TextDescription</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>ProjectSourceKey</t>
   </si>
 </sst>
 </file>
@@ -372,20 +372,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
regenerated stagingtemplate files after meerkat db changes
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Activity.xlsx
+++ b/StagingTemplates/Staging.Activity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnicoloud\Documents\My Docs\Meerkat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Aphelion\Clients\Aphelion\Meerkat\generate staging templates macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>For internal use only. Do not fill in or change</t>
   </si>
   <si>
     <t>Activity_ID</t>
+  </si>
+  <si>
+    <t>BusinessKey</t>
   </si>
   <si>
     <t>Code</t>
@@ -373,23 +376,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -407,6 +414,9 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new staging templates generated
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Activity.xlsx
+++ b/StagingTemplates/Staging.Activity.xlsx
@@ -383,12 +383,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
latest templates with re-ordered columns
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Activity.xlsx
+++ b/StagingTemplates/Staging.Activity.xlsx
@@ -35,13 +35,13 @@
     <t>BusinessKey</t>
   </si>
   <si>
+    <t>ProjectBusinessKey</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
     <t>LongName</t>
-  </si>
-  <si>
-    <t>ProjectBusinessKey</t>
   </si>
   <si>
     <t>ShortName</t>

</xml_diff>

<commit_message>
staging templates updated with database changes - framework and impact
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Activity.xlsx
+++ b/StagingTemplates/Staging.Activity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Aphelion\Clients\Aphelion\Meerkat\generate staging templates macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aphelion\Aphelion\Meerkat\StagingTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25050" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>